<commit_message>
v1.01 updated (update version in file)
</commit_message>
<xml_diff>
--- a/Secure D Web Application Security Test Checklist v1.01.xlsx
+++ b/Secure D Web Application Security Test Checklist v1.01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bankde/Desktop/work/wastc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4E5F22-7818-C743-BCF9-B5F3C3F0BC89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80239C37-8F9E-704F-BA3F-232EAAADFB85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2234,9 +2234,6 @@
       </rPr>
       <t xml:space="preserve"> Incorrect casting between integer, float, boolean.</t>
     </r>
-  </si>
-  <si>
-    <t>Secure D Web Application Security Test Checklist v1.00</t>
   </si>
   <si>
     <t>Insecure usage of browser local storage</t>
@@ -3052,6 +3049,9 @@
 Developer MUST carefully study the framework how it processes the HTTP parameter.
 Do NOT manually concatenate the user input into a server request, JSON, or XML creation. For frontend developer, using framework request form is recommended. For backend developer, using secure template is recommended.
 The developer could carefully study the control characters and manually escape them before HTTP requests, JSON, or XML creation. The control characters can be varied and can be easily missed. This option should only be done when there is no other solutions.</t>
+  </si>
+  <si>
+    <t>Secure D Web Application Security Test Checklist v1.01</t>
   </si>
 </sst>
 </file>
@@ -4626,7 +4626,7 @@
   <dimension ref="A1:IV8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4682,7 +4682,7 @@
     <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
-        <v>259</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4757,7 +4757,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -4777,10 +4777,10 @@
         <v>15</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D4" s="35" t="s">
         <v>265</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>266</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -4796,10 +4796,10 @@
         <v>167</v>
       </c>
       <c r="C5" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>267</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>268</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -4815,10 +4815,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -4834,10 +4834,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
@@ -4853,10 +4853,10 @@
         <v>20</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -4872,10 +4872,10 @@
         <v>22</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
@@ -4906,7 +4906,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>168</v>
@@ -4925,10 +4925,10 @@
         <v>27</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
@@ -4944,10 +4944,10 @@
         <v>224</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -5028,7 +5028,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -5048,10 +5048,10 @@
         <v>31</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -5067,10 +5067,10 @@
         <v>33</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -5127,7 +5127,7 @@
         <v>226</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -5155,10 +5155,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D10" s="37" t="s">
         <v>16</v>
@@ -5177,7 +5177,7 @@
         <v>39</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D11" s="37" t="s">
         <v>16</v>
@@ -5196,7 +5196,7 @@
         <v>41</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D12" s="37" t="s">
         <v>16</v>
@@ -5215,10 +5215,10 @@
         <v>43</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -5234,10 +5234,10 @@
         <v>45</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
@@ -5249,10 +5249,10 @@
       <c r="A15" s="14"/>
       <c r="B15" s="26"/>
       <c r="C15" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
@@ -5268,10 +5268,10 @@
         <v>47</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
@@ -5287,10 +5287,10 @@
         <v>48</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
@@ -5306,10 +5306,10 @@
         <v>50</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -5325,10 +5325,10 @@
         <v>52</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -5359,10 +5359,10 @@
         <v>54</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
@@ -5378,10 +5378,10 @@
         <v>55</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
@@ -5394,10 +5394,10 @@
         <v>17</v>
       </c>
       <c r="B23" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>261</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>262</v>
       </c>
       <c r="D23" s="37" t="s">
         <v>16</v>
@@ -5405,7 +5405,7 @@
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -5481,7 +5481,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -5754,7 +5754,7 @@
       <c r="A19" s="20"/>
       <c r="B19" s="26"/>
       <c r="C19" s="22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>16</v>
@@ -5769,15 +5769,15 @@
       <c r="A20" s="20"/>
       <c r="B20" s="26"/>
       <c r="C20" s="40" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="140" x14ac:dyDescent="0.15">
@@ -6065,7 +6065,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -6085,10 +6085,10 @@
         <v>98</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -6104,10 +6104,10 @@
         <v>99</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -6123,10 +6123,10 @@
         <v>101</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -6142,10 +6142,10 @@
         <v>103</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
@@ -6161,10 +6161,10 @@
         <v>105</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -6180,10 +6180,10 @@
         <v>107</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
@@ -6216,10 +6216,10 @@
         <v>110</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
@@ -6246,10 +6246,10 @@
       <c r="A13" s="20"/>
       <c r="B13" s="26"/>
       <c r="C13" s="22" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -6284,10 +6284,10 @@
         <v>115</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
@@ -6303,10 +6303,10 @@
         <v>116</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
@@ -6341,10 +6341,10 @@
         <v>119</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -6360,10 +6360,10 @@
         <v>121</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -6417,7 +6417,7 @@
         <v>126</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D22" s="33" t="s">
         <v>16</v>
@@ -6425,7 +6425,7 @@
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="168" x14ac:dyDescent="0.15">
@@ -6433,16 +6433,16 @@
         <v>17</v>
       </c>
       <c r="B23" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>324</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>325</v>
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="84" x14ac:dyDescent="0.15">
@@ -6472,10 +6472,10 @@
         <v>127</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
@@ -6491,10 +6491,10 @@
         <v>129</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
@@ -6510,10 +6510,10 @@
         <v>131</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
@@ -6529,10 +6529,10 @@
         <v>133</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
@@ -6548,10 +6548,10 @@
         <v>135</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
@@ -6719,7 +6719,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
@@ -6739,7 +6739,7 @@
         <v>144</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>16</v>
@@ -6918,7 +6918,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>

</xml_diff>